<commit_message>
DC : Updated time sheet Updated Combined Group Timesheets
</commit_message>
<xml_diff>
--- a/documentation/Timesheets/RUP Project Delivery.xlsx
+++ b/documentation/Timesheets/RUP Project Delivery.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MyAdminSorted\Repository\ELEN7046_Group2_2016\documentation\Timesheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="7995"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>Inception Phase</t>
   </si>
@@ -148,6 +153,9 @@
   </si>
   <si>
     <t>Environment</t>
+  </si>
+  <si>
+    <t>Research</t>
   </si>
 </sst>
 </file>
@@ -311,6 +319,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -358,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,7 +404,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,9 +613,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C6" sqref="C6"/>
     </sheetView>
@@ -695,39 +706,35 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -735,16 +742,18 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -753,80 +762,82 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>39</v>
+      <c r="A10" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -834,92 +845,88 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>30</v>
@@ -930,15 +937,15 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>30</v>
@@ -949,24 +956,43 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Individual Report - 90% Complete
</commit_message>
<xml_diff>
--- a/documentation/Timesheets/RUP Project Delivery.xlsx
+++ b/documentation/Timesheets/RUP Project Delivery.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MyAdminSorted\Repository\ELEN7046_Group2_2016\documentation\Timesheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -369,7 +364,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +399,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,7 +612,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>

</xml_diff>